<commit_message>
added actors as descriptorsa
</commit_message>
<xml_diff>
--- a/anton_import_test_data.xlsx
+++ b/anton_import_test_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16960"/>
+    <workbookView xWindow="540" yWindow="460" windowWidth="26720" windowHeight="16960"/>
   </bookViews>
   <sheets>
     <sheet name="import_tabelle" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="172">
   <si>
     <t>parent</t>
   </si>
@@ -572,6 +572,15 @@
   </si>
   <si>
     <t>anton::1911-01-01</t>
+  </si>
+  <si>
+    <t>schlagworte_names</t>
+  </si>
+  <si>
+    <t>Kränzle, Andreas; Meyerhans, Andreas</t>
+  </si>
+  <si>
+    <t>Helg, Pater Lukas</t>
   </si>
 </sst>
 </file>
@@ -623,7 +632,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="62">
+  <cellStyleXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -673,6 +682,36 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -693,7 +732,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="62">
+  <cellStyles count="92">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -725,6 +764,21 @@
     <cellStyle name="Besuchter Link" xfId="57" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="59" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="91" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -755,6 +809,21 @@
     <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="66" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="68" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="70" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="72" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="74" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="76" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="78" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="80" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="82" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="84" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="88" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="90" builtinId="8" hidden="1"/>
     <cellStyle name="Stand." xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1057,11 +1126,11 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AQ20"/>
+  <dimension ref="A1:AR20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AL1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AQ20" sqref="AQ20"/>
+      <selection pane="bottomLeft" activeCell="U7" sqref="U7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1084,29 +1153,31 @@
     <col min="16" max="16" width="7" bestFit="1" customWidth="1"/>
     <col min="17" max="18" width="21" customWidth="1"/>
     <col min="19" max="19" width="21" style="1" customWidth="1"/>
-    <col min="20" max="21" width="14" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14" customWidth="1"/>
-    <col min="23" max="23" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="31.6640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="29.5" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="38.83203125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="36" max="37" width="27" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="33" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14" customWidth="1"/>
+    <col min="22" max="22" width="14" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14" customWidth="1"/>
+    <col min="24" max="24" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="31.6640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="29.5" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="38.83203125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="37" max="38" width="27" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="33" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="37.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1168,76 +1239,79 @@
         <v>16</v>
       </c>
       <c r="U1" t="s">
+        <v>169</v>
+      </c>
+      <c r="V1" t="s">
         <v>17</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>149</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>18</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>71</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>19</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>20</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>21</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>108</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>22</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>23</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>72</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>73</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>69</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>74</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>75</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>106</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>24</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>105</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>25</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>70</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>76</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>107</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>102</v>
       </c>
@@ -1286,17 +1360,17 @@
       <c r="T2" t="s">
         <v>32</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>33</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>34</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>102</v>
       </c>
@@ -1337,20 +1411,20 @@
       <c r="T3" t="s">
         <v>50</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V3" t="s">
         <v>33</v>
       </c>
-      <c r="W3" t="s">
+      <c r="X3" t="s">
         <v>43</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AA3" t="s">
         <v>39</v>
       </c>
-      <c r="AE3" t="s">
+      <c r="AF3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>102</v>
       </c>
@@ -1397,17 +1471,17 @@
       <c r="T4" t="s">
         <v>124</v>
       </c>
-      <c r="U4" t="s">
+      <c r="V4" t="s">
         <v>33</v>
       </c>
-      <c r="W4" t="s">
+      <c r="X4" t="s">
         <v>125</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="AA4" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>127</v>
       </c>
@@ -1455,16 +1529,19 @@
         <v>92</v>
       </c>
       <c r="U5" t="s">
+        <v>170</v>
+      </c>
+      <c r="V5" t="s">
         <v>33</v>
       </c>
-      <c r="W5" t="s">
+      <c r="X5" t="s">
         <v>93</v>
       </c>
-      <c r="Z5" t="s">
+      <c r="AA5" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>127</v>
       </c>
@@ -1510,10 +1587,13 @@
         <v>100</v>
       </c>
       <c r="U6" t="s">
+        <v>171</v>
+      </c>
+      <c r="V6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>114</v>
       </c>
@@ -1558,14 +1638,14 @@
       <c r="T7" t="s">
         <v>135</v>
       </c>
-      <c r="U7" t="s">
+      <c r="V7" t="s">
         <v>33</v>
       </c>
-      <c r="Z7" t="s">
+      <c r="AA7" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="8" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>114</v>
       </c>
@@ -1610,14 +1690,14 @@
       <c r="T8" t="s">
         <v>135</v>
       </c>
-      <c r="U8" t="s">
+      <c r="V8" t="s">
         <v>84</v>
       </c>
-      <c r="Z8" t="s">
+      <c r="AA8" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="9" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>114</v>
       </c>
@@ -1662,14 +1742,14 @@
       <c r="T9" t="s">
         <v>135</v>
       </c>
-      <c r="U9" t="s">
+      <c r="V9" t="s">
         <v>84</v>
       </c>
-      <c r="Z9" t="s">
+      <c r="AA9" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="10" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>114</v>
       </c>
@@ -1714,14 +1794,14 @@
       <c r="T10" t="s">
         <v>135</v>
       </c>
-      <c r="U10" t="s">
+      <c r="V10" t="s">
         <v>84</v>
       </c>
-      <c r="Z10" t="s">
+      <c r="AA10" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="11" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>128</v>
       </c>
@@ -1766,17 +1846,17 @@
       <c r="T11" t="s">
         <v>118</v>
       </c>
-      <c r="U11" t="s">
+      <c r="V11" t="s">
         <v>86</v>
       </c>
-      <c r="W11" t="s">
+      <c r="X11" t="s">
         <v>120</v>
       </c>
-      <c r="Z11" t="s">
+      <c r="AA11" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="12" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>103</v>
       </c>
@@ -1825,71 +1905,71 @@
       <c r="T12" t="s">
         <v>52</v>
       </c>
-      <c r="U12" t="s">
+      <c r="V12" t="s">
         <v>33</v>
       </c>
-      <c r="W12" t="s">
+      <c r="X12" t="s">
         <v>51</v>
       </c>
-      <c r="X12" t="s">
+      <c r="Y12" t="s">
         <v>79</v>
       </c>
-      <c r="Y12" t="s">
+      <c r="Z12" t="s">
         <v>53</v>
       </c>
-      <c r="Z12" t="s">
+      <c r="AA12" t="s">
         <v>82</v>
       </c>
-      <c r="AA12" t="s">
+      <c r="AB12" t="s">
         <v>54</v>
       </c>
-      <c r="AB12" t="s">
+      <c r="AC12" t="s">
         <v>55</v>
       </c>
-      <c r="AC12" t="s">
+      <c r="AD12" t="s">
         <v>56</v>
       </c>
-      <c r="AD12" t="s">
+      <c r="AE12" t="s">
         <v>57</v>
       </c>
-      <c r="AE12" t="s">
+      <c r="AF12" t="s">
         <v>58</v>
       </c>
-      <c r="AF12" t="s">
+      <c r="AG12" t="s">
         <v>77</v>
       </c>
-      <c r="AG12" t="s">
+      <c r="AH12" t="s">
         <v>59</v>
       </c>
-      <c r="AH12" t="s">
+      <c r="AI12" t="s">
         <v>60</v>
       </c>
-      <c r="AI12" t="s">
+      <c r="AJ12" t="s">
         <v>64</v>
       </c>
-      <c r="AJ12" t="s">
+      <c r="AK12" t="s">
         <v>61</v>
       </c>
-      <c r="AK12" t="s">
+      <c r="AL12" t="s">
         <v>62</v>
       </c>
-      <c r="AL12" t="s">
+      <c r="AM12" t="s">
         <v>63</v>
       </c>
-      <c r="AM12" t="s">
+      <c r="AN12" t="s">
         <v>65</v>
       </c>
-      <c r="AN12" t="s">
+      <c r="AO12" t="s">
         <v>78</v>
       </c>
-      <c r="AO12" t="s">
+      <c r="AP12" t="s">
         <v>66</v>
       </c>
-      <c r="AP12" t="s">
+      <c r="AQ12" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>103</v>
       </c>
@@ -1926,11 +2006,11 @@
       <c r="T13" t="s">
         <v>52</v>
       </c>
-      <c r="U13" t="s">
+      <c r="V13" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="14" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>103</v>
       </c>
@@ -1967,11 +2047,11 @@
       <c r="T14" t="s">
         <v>52</v>
       </c>
-      <c r="U14" t="s">
+      <c r="V14" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>103</v>
       </c>
@@ -2002,14 +2082,14 @@
       <c r="P15">
         <v>0</v>
       </c>
-      <c r="U15" t="s">
+      <c r="V15" t="s">
         <v>33</v>
       </c>
-      <c r="W15" t="s">
+      <c r="X15" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="16" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>103</v>
       </c>
@@ -2043,14 +2123,14 @@
       <c r="Q16" t="s">
         <v>156</v>
       </c>
-      <c r="U16" t="s">
+      <c r="V16" t="s">
         <v>33</v>
       </c>
-      <c r="V16">
+      <c r="W16">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>103</v>
       </c>
@@ -2084,11 +2164,11 @@
       <c r="P17">
         <v>0</v>
       </c>
-      <c r="U17" t="s">
+      <c r="V17" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>103</v>
       </c>
@@ -2122,11 +2202,11 @@
       <c r="Q18" t="s">
         <v>159</v>
       </c>
-      <c r="U18" t="s">
+      <c r="V18" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>103</v>
       </c>
@@ -2160,11 +2240,11 @@
       <c r="Q19" t="s">
         <v>162</v>
       </c>
-      <c r="U19" t="s">
+      <c r="V19" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>103</v>
       </c>
@@ -2195,10 +2275,10 @@
       <c r="P20">
         <v>0</v>
       </c>
-      <c r="U20" t="s">
+      <c r="V20" t="s">
         <v>33</v>
       </c>
-      <c r="AQ20" t="s">
+      <c r="AR20" t="s">
         <v>168</v>
       </c>
     </row>

</xml_diff>